<commit_message>
texto consolidación tema 2 grado 08
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/esqueletoGuion_MA_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/esqueletoGuion_MA_08_02_CO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="12240" windowHeight="9240" tabRatio="729" activeTab="1"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="12240" windowHeight="9240" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="92">
   <si>
     <t>FICHA</t>
   </si>
@@ -1833,7 +1833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -2547,10 +2547,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I67" sqref="I67"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3037,46 +3037,46 @@
         <v>30</v>
       </c>
       <c r="E26" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="38"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="15"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="18" t="s">
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="I26" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="62"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
+      <c r="I27" s="15" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="E28" s="20" t="s">
+      <c r="B28" s="64" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="20" t="s">
         <v>25</v>
       </c>
+      <c r="D28" s="62"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
       <c r="H28" s="21"/>
@@ -3089,7 +3089,7 @@
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="64" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E29" s="20" t="s">
         <v>25</v>
@@ -3106,7 +3106,7 @@
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
       <c r="D30" s="64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>25</v>
@@ -3123,12 +3123,12 @@
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
       <c r="D31" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E31" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F31" s="62"/>
+      <c r="F31" s="20"/>
       <c r="G31" s="20"/>
       <c r="H31" s="21"/>
       <c r="I31" s="21"/>
@@ -3142,17 +3142,13 @@
       <c r="D32" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="41" t="s">
-        <v>27</v>
+      <c r="E32" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="F32" s="62"/>
       <c r="G32" s="20"/>
-      <c r="H32" s="63" t="s">
-        <v>46</v>
-      </c>
-      <c r="I32" s="21" t="s">
-        <v>23</v>
-      </c>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
@@ -3164,7 +3160,7 @@
         <v>78</v>
       </c>
       <c r="E33" s="41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F33" s="62"/>
       <c r="G33" s="20"/>
@@ -3172,7 +3168,7 @@
         <v>46</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3182,76 +3178,74 @@
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
       <c r="D34" s="64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E34" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="F34" s="19"/>
+        <v>28</v>
+      </c>
+      <c r="F34" s="62"/>
       <c r="G34" s="20"/>
       <c r="H34" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="I34" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="62"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="21"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" s="19"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="I34" s="21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="B35" s="68" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="70"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="5"/>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="68" t="s">
-        <v>81</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="5"/>
+      <c r="I36" s="21" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="68" t="s">
-        <v>81</v>
-      </c>
-      <c r="E37" s="39" t="s">
-        <v>27</v>
-      </c>
+      <c r="B37" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="23"/>
+      <c r="E37" s="24"/>
       <c r="F37" s="24"/>
       <c r="G37" s="24"/>
-      <c r="H37" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="I37" s="25" t="s">
-        <v>23</v>
-      </c>
+      <c r="H37" s="70"/>
+      <c r="I37" s="25"/>
       <c r="J37" s="5"/>
     </row>
     <row r="38" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3259,12 +3253,12 @@
         <v>64</v>
       </c>
       <c r="B38" s="23"/>
-      <c r="C38" s="26"/>
+      <c r="C38" s="24"/>
       <c r="D38" s="68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F38" s="24"/>
       <c r="G38" s="24"/>
@@ -3279,15 +3273,19 @@
       <c r="B39" s="23"/>
       <c r="C39" s="26"/>
       <c r="D39" s="68" t="s">
-        <v>82</v>
-      </c>
-      <c r="E39" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="F39" s="69"/>
+        <v>81</v>
+      </c>
+      <c r="E39" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" s="24"/>
       <c r="G39" s="24"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
+      <c r="H39" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="I39" s="25" t="s">
+        <v>23</v>
+      </c>
       <c r="J39" s="5"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3296,15 +3294,15 @@
       </c>
       <c r="B40" s="23"/>
       <c r="C40" s="26"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="68" t="s">
-        <v>83</v>
-      </c>
-      <c r="G40" s="24" t="s">
+      <c r="D40" s="68" t="s">
+        <v>82</v>
+      </c>
+      <c r="E40" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="H40" s="40"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="25"/>
       <c r="I40" s="25"/>
       <c r="J40" s="5"/>
     </row>
@@ -3314,15 +3312,15 @@
       </c>
       <c r="B41" s="23"/>
       <c r="C41" s="26"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="68" t="s">
-        <v>84</v>
-      </c>
-      <c r="G41" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="H41" s="71"/>
+      <c r="D41" s="68" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F41" s="69"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="25"/>
       <c r="I41" s="25"/>
       <c r="J41" s="5"/>
     </row>
@@ -3332,15 +3330,15 @@
       </c>
       <c r="B42" s="23"/>
       <c r="C42" s="26"/>
-      <c r="D42" s="23"/>
+      <c r="D42" s="24"/>
       <c r="E42" s="24"/>
       <c r="F42" s="68" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G42" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="H42" s="28"/>
+      <c r="H42" s="40"/>
       <c r="I42" s="25"/>
       <c r="J42" s="5"/>
     </row>
@@ -3350,15 +3348,15 @@
       </c>
       <c r="B43" s="23"/>
       <c r="C43" s="26"/>
-      <c r="D43" s="69"/>
-      <c r="E43" s="39"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="24"/>
       <c r="F43" s="68" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G43" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="H43" s="40"/>
+        <v>25</v>
+      </c>
+      <c r="H43" s="71"/>
       <c r="I43" s="25"/>
       <c r="J43" s="5"/>
     </row>
@@ -3366,39 +3364,35 @@
       <c r="A44" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B44" s="69"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="23"/>
       <c r="E44" s="24"/>
       <c r="F44" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="G44" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="H44" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="I44" s="25" t="s">
-        <v>23</v>
-      </c>
+      <c r="G44" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H44" s="28"/>
+      <c r="I44" s="25"/>
       <c r="J44" s="5"/>
     </row>
     <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="69"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="E45" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="F45" s="23"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="25"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="69"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="G45" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H45" s="40"/>
       <c r="I45" s="25"/>
       <c r="J45" s="5"/>
     </row>
@@ -3407,17 +3401,21 @@
         <v>64</v>
       </c>
       <c r="B46" s="69"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="E46" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="F46" s="23"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="25"/>
-      <c r="I46" s="25"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="G46" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="H46" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="I46" s="25" t="s">
+        <v>23</v>
+      </c>
       <c r="J46" s="5"/>
     </row>
     <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3426,15 +3424,15 @@
       </c>
       <c r="B47" s="69"/>
       <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="68" t="s">
-        <v>87</v>
-      </c>
-      <c r="G47" s="24" t="s">
+      <c r="D47" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="E47" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="H47" s="40"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="25"/>
       <c r="I47" s="25"/>
       <c r="J47" s="5"/>
     </row>
@@ -3442,17 +3440,17 @@
       <c r="A48" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="69"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="G48" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="H48" s="28"/>
+      <c r="B48" s="69"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="E48" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48" s="23"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="25"/>
       <c r="I48" s="25"/>
       <c r="J48" s="5"/>
     </row>
@@ -3460,17 +3458,17 @@
       <c r="A49" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B49" s="23"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="69"/>
+      <c r="B49" s="69"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
       <c r="E49" s="24"/>
       <c r="F49" s="68" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G49" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="H49" s="25"/>
+      <c r="H49" s="40"/>
       <c r="I49" s="25"/>
       <c r="J49" s="5"/>
     </row>
@@ -3480,15 +3478,15 @@
       </c>
       <c r="B50" s="23"/>
       <c r="C50" s="26"/>
-      <c r="D50" s="71"/>
+      <c r="D50" s="69"/>
       <c r="E50" s="24"/>
       <c r="F50" s="68" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G50" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="H50" s="25"/>
+        <v>25</v>
+      </c>
+      <c r="H50" s="28"/>
       <c r="I50" s="25"/>
       <c r="J50" s="5"/>
     </row>
@@ -3506,7 +3504,7 @@
       <c r="G51" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="H51" s="28"/>
+      <c r="H51" s="25"/>
       <c r="I51" s="25"/>
       <c r="J51" s="5"/>
     </row>
@@ -3516,7 +3514,7 @@
       </c>
       <c r="B52" s="23"/>
       <c r="C52" s="26"/>
-      <c r="D52" s="69"/>
+      <c r="D52" s="71"/>
       <c r="E52" s="24"/>
       <c r="F52" s="68" t="s">
         <v>89</v>
@@ -3524,7 +3522,7 @@
       <c r="G52" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H52" s="28"/>
+      <c r="H52" s="25"/>
       <c r="I52" s="25"/>
       <c r="J52" s="5"/>
     </row>
@@ -3539,15 +3537,11 @@
       <c r="F53" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="G53" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="H53" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="I53" s="25" t="s">
-        <v>24</v>
-      </c>
+      <c r="G53" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H53" s="28"/>
+      <c r="I53" s="25"/>
       <c r="J53" s="5"/>
     </row>
     <row r="54" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3555,21 +3549,17 @@
         <v>64</v>
       </c>
       <c r="B54" s="23"/>
-      <c r="C54" s="24"/>
+      <c r="C54" s="26"/>
       <c r="D54" s="69"/>
-      <c r="E54" s="43"/>
+      <c r="E54" s="24"/>
       <c r="F54" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="G54" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="H54" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="I54" s="25" t="s">
-        <v>24</v>
-      </c>
+      <c r="G54" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H54" s="28"/>
+      <c r="I54" s="25"/>
       <c r="J54" s="5"/>
     </row>
     <row r="55" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3577,17 +3567,21 @@
         <v>64</v>
       </c>
       <c r="B55" s="23"/>
-      <c r="C55" s="24"/>
+      <c r="C55" s="26"/>
       <c r="D55" s="69"/>
-      <c r="E55" s="39"/>
+      <c r="E55" s="24"/>
       <c r="F55" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="G55" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="H55" s="28"/>
-      <c r="I55" s="25"/>
+        <v>89</v>
+      </c>
+      <c r="G55" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="H55" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="I55" s="25" t="s">
+        <v>24</v>
+      </c>
       <c r="J55" s="5"/>
     </row>
     <row r="56" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3597,32 +3591,36 @@
       <c r="B56" s="23"/>
       <c r="C56" s="24"/>
       <c r="D56" s="69"/>
-      <c r="E56" s="39"/>
+      <c r="E56" s="43"/>
       <c r="F56" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="G56" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="H56" s="27"/>
-      <c r="I56" s="25"/>
+        <v>89</v>
+      </c>
+      <c r="G56" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="H56" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="I56" s="25" t="s">
+        <v>24</v>
+      </c>
       <c r="J56" s="5"/>
     </row>
     <row r="57" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B57" s="69"/>
+      <c r="B57" s="23"/>
       <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
+      <c r="D57" s="69"/>
+      <c r="E57" s="39"/>
       <c r="F57" s="68" t="s">
         <v>90</v>
       </c>
       <c r="G57" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="H57" s="25"/>
+      <c r="H57" s="28"/>
       <c r="I57" s="25"/>
       <c r="J57" s="5"/>
     </row>
@@ -3630,17 +3628,17 @@
       <c r="A58" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B58" s="69"/>
+      <c r="B58" s="23"/>
       <c r="C58" s="24"/>
-      <c r="D58" s="27"/>
-      <c r="E58" s="24"/>
+      <c r="D58" s="69"/>
+      <c r="E58" s="39"/>
       <c r="F58" s="68" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="G58" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="H58" s="25"/>
+        <v>29</v>
+      </c>
+      <c r="H58" s="27"/>
       <c r="I58" s="25"/>
       <c r="J58" s="5"/>
     </row>
@@ -3648,44 +3646,36 @@
       <c r="A59" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="69"/>
+      <c r="B59" s="69"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
       <c r="E59" s="24"/>
       <c r="F59" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="G59" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="H59" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="I59" s="25" t="s">
-        <v>23</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="G59" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H59" s="25"/>
+      <c r="I59" s="25"/>
       <c r="J59" s="5"/>
     </row>
     <row r="60" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B60" s="23"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="69"/>
+      <c r="B60" s="69"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="27"/>
       <c r="E60" s="24"/>
       <c r="F60" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="G60" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="H60" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="I60" s="25" t="s">
-        <v>24</v>
-      </c>
+      <c r="G60" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H60" s="25"/>
+      <c r="I60" s="25"/>
       <c r="J60" s="5"/>
     </row>
     <row r="61" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3694,202 +3684,233 @@
       </c>
       <c r="B61" s="23"/>
       <c r="C61" s="26"/>
-      <c r="D61" s="68" t="s">
+      <c r="D61" s="69"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="G61" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="H61" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="I61" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="J61" s="5"/>
+    </row>
+    <row r="62" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="23"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="69"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="G62" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="H62" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="I62" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="J62" s="5"/>
+    </row>
+    <row r="63" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" s="23"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="E61" s="39" t="s">
+      <c r="E63" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F63" s="68"/>
+      <c r="G63" s="39"/>
+      <c r="H63" s="28"/>
+      <c r="I63" s="25"/>
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="23"/>
+      <c r="C64" s="26"/>
+      <c r="D64" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="E64" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="F61" s="24"/>
-      <c r="G61" s="24"/>
-      <c r="H61" s="29" t="s">
+      <c r="F64" s="24"/>
+      <c r="G64" s="24"/>
+      <c r="H64" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="I61" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="J61" s="5"/>
-    </row>
-    <row r="62" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="B62" s="72" t="s">
+      <c r="I64" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="J64" s="5"/>
+    </row>
+    <row r="65" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="C62" s="44" t="s">
+      <c r="C65" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="D62" s="73"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="73"/>
-      <c r="G62" s="30"/>
-      <c r="H62" s="32" t="s">
+      <c r="D65" s="73"/>
+      <c r="E65" s="30"/>
+      <c r="F65" s="73"/>
+      <c r="G65" s="30"/>
+      <c r="H65" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="I62" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="J62" s="5"/>
-    </row>
-    <row r="63" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="B63" s="72" t="s">
+      <c r="I65" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="J65" s="5"/>
+    </row>
+    <row r="66" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B66" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="C63" s="44" t="s">
+      <c r="C66" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="D63" s="73"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="73"/>
-      <c r="G63" s="44"/>
-      <c r="H63" s="32" t="s">
+      <c r="D66" s="73"/>
+      <c r="E66" s="30"/>
+      <c r="F66" s="73"/>
+      <c r="G66" s="44"/>
+      <c r="H66" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="I63" s="31" t="s">
+      <c r="I66" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="J63" s="5"/>
-    </row>
-    <row r="64" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="B64" s="72" t="s">
+      <c r="J66" s="5"/>
+    </row>
+    <row r="67" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B67" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="C64" s="44" t="s">
+      <c r="C67" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="D64" s="73"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="30"/>
-      <c r="G64" s="30"/>
-      <c r="H64" s="32" t="s">
+      <c r="D67" s="73"/>
+      <c r="E67" s="30"/>
+      <c r="F67" s="30"/>
+      <c r="G67" s="30"/>
+      <c r="H67" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="I64" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="J64" s="5"/>
-    </row>
-    <row r="65" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="B65" s="74" t="s">
+      <c r="I67" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="J67" s="5"/>
+    </row>
+    <row r="68" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B68" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="C65" s="33" t="s">
+      <c r="C68" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D65" s="75"/>
-      <c r="E65" s="35"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="34"/>
-      <c r="H65" s="54"/>
-      <c r="I65" s="35"/>
-      <c r="J65" s="5"/>
-    </row>
-    <row r="66" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="B66" s="74" t="s">
+      <c r="D68" s="75"/>
+      <c r="E68" s="35"/>
+      <c r="F68" s="75"/>
+      <c r="G68" s="34"/>
+      <c r="H68" s="54"/>
+      <c r="I68" s="35"/>
+      <c r="J68" s="5"/>
+    </row>
+    <row r="69" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B69" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="C66" s="33" t="s">
+      <c r="C69" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D66" s="75"/>
-      <c r="E66" s="34"/>
-      <c r="F66" s="75"/>
-      <c r="G66" s="34"/>
-      <c r="H66" s="76" t="s">
+      <c r="D69" s="75"/>
+      <c r="E69" s="34"/>
+      <c r="F69" s="75"/>
+      <c r="G69" s="34"/>
+      <c r="H69" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="I66" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="J66" s="5"/>
-    </row>
-    <row r="67" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="5"/>
-      <c r="B67" s="45"/>
-      <c r="C67" s="48"/>
-      <c r="D67" s="48"/>
-      <c r="E67" s="48"/>
-      <c r="F67" s="48"/>
-      <c r="G67" s="61"/>
-      <c r="H67" s="50"/>
-      <c r="J67" s="5"/>
-    </row>
-    <row r="68" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
-      <c r="B68" s="45"/>
-      <c r="C68" s="48"/>
-      <c r="D68" s="60"/>
-      <c r="E68" s="61"/>
-      <c r="F68" s="48"/>
-      <c r="G68" s="48"/>
-      <c r="H68" s="50"/>
-      <c r="J68" s="5"/>
-    </row>
-    <row r="69" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
-      <c r="B69" s="60"/>
-      <c r="C69" s="61"/>
-      <c r="D69" s="45"/>
-      <c r="E69" s="48"/>
-      <c r="F69" s="48"/>
-      <c r="G69" s="48"/>
-      <c r="H69" s="50"/>
+      <c r="I69" s="35" t="s">
+        <v>23</v>
+      </c>
       <c r="J69" s="5"/>
     </row>
     <row r="70" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="45"/>
-      <c r="C70" s="46"/>
-      <c r="D70" s="45"/>
+      <c r="C70" s="48"/>
+      <c r="D70" s="48"/>
       <c r="E70" s="48"/>
       <c r="F70" s="48"/>
-      <c r="G70" s="48"/>
-      <c r="H70" s="5"/>
+      <c r="G70" s="61"/>
+      <c r="H70" s="50"/>
       <c r="J70" s="5"/>
     </row>
     <row r="71" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="45"/>
-      <c r="C71" s="46"/>
-      <c r="D71" s="47"/>
-      <c r="E71" s="48"/>
+      <c r="C71" s="48"/>
+      <c r="D71" s="60"/>
+      <c r="E71" s="61"/>
       <c r="F71" s="48"/>
       <c r="G71" s="48"/>
-      <c r="H71" s="5"/>
+      <c r="H71" s="50"/>
       <c r="J71" s="5"/>
     </row>
     <row r="72" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
-      <c r="B72" s="45"/>
-      <c r="C72" s="46"/>
-      <c r="D72" s="47"/>
+      <c r="B72" s="60"/>
+      <c r="C72" s="61"/>
+      <c r="D72" s="45"/>
       <c r="E72" s="48"/>
-      <c r="F72" s="47"/>
+      <c r="F72" s="48"/>
       <c r="G72" s="48"/>
-      <c r="H72" s="5"/>
+      <c r="H72" s="50"/>
+      <c r="J72" s="5"/>
     </row>
     <row r="73" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="45"/>
       <c r="C73" s="46"/>
-      <c r="D73" s="47"/>
+      <c r="D73" s="45"/>
       <c r="E73" s="48"/>
-      <c r="F73" s="47"/>
+      <c r="F73" s="48"/>
       <c r="G73" s="48"/>
-      <c r="H73" s="49"/>
+      <c r="H73" s="5"/>
+      <c r="J73" s="5"/>
     </row>
     <row r="74" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
@@ -3900,12 +3921,13 @@
       <c r="F74" s="48"/>
       <c r="G74" s="48"/>
       <c r="H74" s="5"/>
+      <c r="J74" s="5"/>
     </row>
     <row r="75" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="45"/>
       <c r="C75" s="46"/>
-      <c r="D75" s="48"/>
+      <c r="D75" s="47"/>
       <c r="E75" s="48"/>
       <c r="F75" s="47"/>
       <c r="G75" s="48"/>
@@ -3915,19 +3937,19 @@
       <c r="A76" s="5"/>
       <c r="B76" s="45"/>
       <c r="C76" s="46"/>
-      <c r="D76" s="48"/>
+      <c r="D76" s="47"/>
       <c r="E76" s="48"/>
       <c r="F76" s="47"/>
       <c r="G76" s="48"/>
-      <c r="H76" s="5"/>
+      <c r="H76" s="49"/>
     </row>
     <row r="77" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="45"/>
       <c r="C77" s="46"/>
-      <c r="D77" s="48"/>
+      <c r="D77" s="47"/>
       <c r="E77" s="48"/>
-      <c r="F77" s="45"/>
+      <c r="F77" s="48"/>
       <c r="G77" s="48"/>
       <c r="H77" s="5"/>
     </row>
@@ -3937,7 +3959,7 @@
       <c r="C78" s="46"/>
       <c r="D78" s="48"/>
       <c r="E78" s="48"/>
-      <c r="F78" s="45"/>
+      <c r="F78" s="47"/>
       <c r="G78" s="48"/>
       <c r="H78" s="5"/>
     </row>
@@ -3947,69 +3969,99 @@
       <c r="C79" s="46"/>
       <c r="D79" s="48"/>
       <c r="E79" s="48"/>
-      <c r="F79" s="45"/>
+      <c r="F79" s="47"/>
       <c r="G79" s="48"/>
-      <c r="H79" s="50"/>
+      <c r="H79" s="5"/>
     </row>
     <row r="80" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="45"/>
       <c r="C80" s="46"/>
-      <c r="D80" s="45"/>
+      <c r="D80" s="48"/>
       <c r="E80" s="48"/>
-      <c r="F80" s="48"/>
+      <c r="F80" s="45"/>
       <c r="G80" s="48"/>
-      <c r="H80" s="50"/>
+      <c r="H80" s="5"/>
     </row>
     <row r="81" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
-      <c r="B81" s="47"/>
+      <c r="B81" s="45"/>
       <c r="C81" s="46"/>
-      <c r="D81" s="45"/>
+      <c r="D81" s="48"/>
       <c r="E81" s="48"/>
-      <c r="F81" s="48"/>
+      <c r="F81" s="45"/>
       <c r="G81" s="48"/>
-      <c r="H81" s="50"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H81" s="5"/>
+    </row>
+    <row r="82" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
-      <c r="B82" s="46"/>
+      <c r="B82" s="45"/>
       <c r="C82" s="46"/>
       <c r="D82" s="48"/>
       <c r="E82" s="48"/>
-      <c r="F82" s="48"/>
+      <c r="F82" s="45"/>
       <c r="G82" s="48"/>
-      <c r="H82" s="5"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H82" s="50"/>
+    </row>
+    <row r="83" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
-      <c r="B83" s="46"/>
+      <c r="B83" s="45"/>
       <c r="C83" s="46"/>
-      <c r="D83" s="48"/>
+      <c r="D83" s="45"/>
       <c r="E83" s="48"/>
       <c r="F83" s="48"/>
       <c r="G83" s="48"/>
-      <c r="H83" s="46"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H83" s="50"/>
+    </row>
+    <row r="84" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
-      <c r="B84" s="46"/>
+      <c r="B84" s="47"/>
       <c r="C84" s="46"/>
-      <c r="D84" s="48"/>
+      <c r="D84" s="45"/>
       <c r="E84" s="48"/>
       <c r="F84" s="48"/>
       <c r="G84" s="48"/>
-      <c r="H84" s="5"/>
+      <c r="H84" s="50"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="51"/>
-      <c r="B85" s="52"/>
-      <c r="C85" s="52"/>
-      <c r="D85" s="53"/>
-      <c r="E85" s="53"/>
-      <c r="F85" s="53"/>
-      <c r="G85" s="53"/>
-      <c r="H85" s="51"/>
+      <c r="A85" s="5"/>
+      <c r="B85" s="46"/>
+      <c r="C85" s="46"/>
+      <c r="D85" s="48"/>
+      <c r="E85" s="48"/>
+      <c r="F85" s="48"/>
+      <c r="G85" s="48"/>
+      <c r="H85" s="5"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="5"/>
+      <c r="B86" s="46"/>
+      <c r="C86" s="46"/>
+      <c r="D86" s="48"/>
+      <c r="E86" s="48"/>
+      <c r="F86" s="48"/>
+      <c r="G86" s="48"/>
+      <c r="H86" s="46"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="5"/>
+      <c r="B87" s="46"/>
+      <c r="C87" s="46"/>
+      <c r="D87" s="48"/>
+      <c r="E87" s="48"/>
+      <c r="F87" s="48"/>
+      <c r="G87" s="48"/>
+      <c r="H87" s="5"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="51"/>
+      <c r="B88" s="52"/>
+      <c r="C88" s="52"/>
+      <c r="D88" s="53"/>
+      <c r="E88" s="53"/>
+      <c r="F88" s="53"/>
+      <c r="G88" s="53"/>
+      <c r="H88" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fórmulas y proyecto tema 2 grado 08
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/esqueletoGuion_MA_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/esqueletoGuion_MA_08_02_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CEN_3F_CDO_PC09\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdgarJosué\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="93">
   <si>
     <t>FICHA</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>Competencias</t>
+  </si>
+  <si>
+    <t>Proyecto</t>
   </si>
 </sst>
 </file>
@@ -2019,10 +2022,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C17"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2198,24 +2201,33 @@
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>23</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="B16" s="15"/>
       <c r="C16" s="58">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="58">
         <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="58">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2237,10 +2249,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2486,31 +2498,37 @@
         <v>21</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
-        <v>23</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="C22"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C28" s="6"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="51"/>
+      <c r="C24" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="6"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
+      <c r="A34" s="51"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
@@ -2522,13 +2540,16 @@
       <c r="A37" s="5"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="58"/>
+      <c r="A38" s="5"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="58"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="58"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="58"/>
     </row>
   </sheetData>
   <sortState ref="A2:C38">
@@ -2547,10 +2568,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J88"/>
+  <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3829,21 +3850,25 @@
       <c r="J67" s="5"/>
     </row>
     <row r="68" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="B68" s="74" t="s">
-        <v>32</v>
-      </c>
-      <c r="C68" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="D68" s="75"/>
-      <c r="E68" s="35"/>
-      <c r="F68" s="75"/>
-      <c r="G68" s="34"/>
-      <c r="H68" s="54"/>
-      <c r="I68" s="35"/>
+      <c r="A68" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B68" s="72" t="s">
+        <v>91</v>
+      </c>
+      <c r="C68" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D68" s="73"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="30"/>
+      <c r="G68" s="30"/>
+      <c r="H68" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="I68" s="31" t="s">
+        <v>23</v>
+      </c>
       <c r="J68" s="5"/>
     </row>
     <row r="69" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3854,48 +3879,55 @@
         <v>32</v>
       </c>
       <c r="C69" s="33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D69" s="75"/>
-      <c r="E69" s="34"/>
+      <c r="E69" s="35"/>
       <c r="F69" s="75"/>
       <c r="G69" s="34"/>
-      <c r="H69" s="76" t="s">
+      <c r="H69" s="54"/>
+      <c r="I69" s="35"/>
+      <c r="J69" s="5"/>
+    </row>
+    <row r="70" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B70" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="C70" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="I69" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="J69" s="5"/>
-    </row>
-    <row r="70" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="5"/>
-      <c r="B70" s="45"/>
-      <c r="C70" s="48"/>
-      <c r="D70" s="48"/>
-      <c r="E70" s="48"/>
-      <c r="F70" s="48"/>
-      <c r="G70" s="61"/>
-      <c r="H70" s="50"/>
+      <c r="D70" s="75"/>
+      <c r="E70" s="34"/>
+      <c r="F70" s="75"/>
+      <c r="G70" s="34"/>
+      <c r="H70" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="I70" s="35" t="s">
+        <v>23</v>
+      </c>
       <c r="J70" s="5"/>
     </row>
     <row r="71" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="45"/>
       <c r="C71" s="48"/>
-      <c r="D71" s="60"/>
-      <c r="E71" s="61"/>
+      <c r="D71" s="48"/>
+      <c r="E71" s="48"/>
       <c r="F71" s="48"/>
-      <c r="G71" s="48"/>
+      <c r="G71" s="61"/>
       <c r="H71" s="50"/>
       <c r="J71" s="5"/>
     </row>
     <row r="72" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
-      <c r="B72" s="60"/>
-      <c r="C72" s="61"/>
-      <c r="D72" s="45"/>
-      <c r="E72" s="48"/>
+      <c r="B72" s="45"/>
+      <c r="C72" s="48"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="61"/>
       <c r="F72" s="48"/>
       <c r="G72" s="48"/>
       <c r="H72" s="50"/>
@@ -3903,20 +3935,20 @@
     </row>
     <row r="73" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
-      <c r="B73" s="45"/>
-      <c r="C73" s="46"/>
+      <c r="B73" s="60"/>
+      <c r="C73" s="61"/>
       <c r="D73" s="45"/>
       <c r="E73" s="48"/>
       <c r="F73" s="48"/>
       <c r="G73" s="48"/>
-      <c r="H73" s="5"/>
+      <c r="H73" s="50"/>
       <c r="J73" s="5"/>
     </row>
     <row r="74" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="45"/>
       <c r="C74" s="46"/>
-      <c r="D74" s="47"/>
+      <c r="D74" s="45"/>
       <c r="E74" s="48"/>
       <c r="F74" s="48"/>
       <c r="G74" s="48"/>
@@ -3929,9 +3961,10 @@
       <c r="C75" s="46"/>
       <c r="D75" s="47"/>
       <c r="E75" s="48"/>
-      <c r="F75" s="47"/>
+      <c r="F75" s="48"/>
       <c r="G75" s="48"/>
       <c r="H75" s="5"/>
+      <c r="J75" s="5"/>
     </row>
     <row r="76" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
@@ -3941,7 +3974,7 @@
       <c r="E76" s="48"/>
       <c r="F76" s="47"/>
       <c r="G76" s="48"/>
-      <c r="H76" s="49"/>
+      <c r="H76" s="5"/>
     </row>
     <row r="77" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
@@ -3949,17 +3982,17 @@
       <c r="C77" s="46"/>
       <c r="D77" s="47"/>
       <c r="E77" s="48"/>
-      <c r="F77" s="48"/>
+      <c r="F77" s="47"/>
       <c r="G77" s="48"/>
-      <c r="H77" s="5"/>
+      <c r="H77" s="49"/>
     </row>
     <row r="78" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="45"/>
       <c r="C78" s="46"/>
-      <c r="D78" s="48"/>
+      <c r="D78" s="47"/>
       <c r="E78" s="48"/>
-      <c r="F78" s="47"/>
+      <c r="F78" s="48"/>
       <c r="G78" s="48"/>
       <c r="H78" s="5"/>
     </row>
@@ -3979,7 +4012,7 @@
       <c r="C80" s="46"/>
       <c r="D80" s="48"/>
       <c r="E80" s="48"/>
-      <c r="F80" s="45"/>
+      <c r="F80" s="47"/>
       <c r="G80" s="48"/>
       <c r="H80" s="5"/>
     </row>
@@ -4001,21 +4034,21 @@
       <c r="E82" s="48"/>
       <c r="F82" s="45"/>
       <c r="G82" s="48"/>
-      <c r="H82" s="50"/>
+      <c r="H82" s="5"/>
     </row>
     <row r="83" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="B83" s="45"/>
       <c r="C83" s="46"/>
-      <c r="D83" s="45"/>
+      <c r="D83" s="48"/>
       <c r="E83" s="48"/>
-      <c r="F83" s="48"/>
+      <c r="F83" s="45"/>
       <c r="G83" s="48"/>
       <c r="H83" s="50"/>
     </row>
     <row r="84" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
-      <c r="B84" s="47"/>
+      <c r="B84" s="45"/>
       <c r="C84" s="46"/>
       <c r="D84" s="45"/>
       <c r="E84" s="48"/>
@@ -4023,15 +4056,15 @@
       <c r="G84" s="48"/>
       <c r="H84" s="50"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
-      <c r="B85" s="46"/>
+      <c r="B85" s="47"/>
       <c r="C85" s="46"/>
-      <c r="D85" s="48"/>
+      <c r="D85" s="45"/>
       <c r="E85" s="48"/>
       <c r="F85" s="48"/>
       <c r="G85" s="48"/>
-      <c r="H85" s="5"/>
+      <c r="H85" s="50"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
@@ -4041,7 +4074,7 @@
       <c r="E86" s="48"/>
       <c r="F86" s="48"/>
       <c r="G86" s="48"/>
-      <c r="H86" s="46"/>
+      <c r="H86" s="5"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
@@ -4051,17 +4084,27 @@
       <c r="E87" s="48"/>
       <c r="F87" s="48"/>
       <c r="G87" s="48"/>
-      <c r="H87" s="5"/>
+      <c r="H87" s="46"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="51"/>
-      <c r="B88" s="52"/>
-      <c r="C88" s="52"/>
-      <c r="D88" s="53"/>
-      <c r="E88" s="53"/>
-      <c r="F88" s="53"/>
-      <c r="G88" s="53"/>
-      <c r="H88" s="51"/>
+      <c r="A88" s="5"/>
+      <c r="B88" s="46"/>
+      <c r="C88" s="46"/>
+      <c r="D88" s="48"/>
+      <c r="E88" s="48"/>
+      <c r="F88" s="48"/>
+      <c r="G88" s="48"/>
+      <c r="H88" s="5"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="51"/>
+      <c r="B89" s="52"/>
+      <c r="C89" s="52"/>
+      <c r="D89" s="53"/>
+      <c r="E89" s="53"/>
+      <c r="F89" s="53"/>
+      <c r="G89" s="53"/>
+      <c r="H89" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>